<commit_message>
Update glutamate and rett syndrome cdkl5.xlsx
</commit_message>
<xml_diff>
--- a/paper/Tables/glutamate and rett syndrome cdkl5.xlsx
+++ b/paper/Tables/glutamate and rett syndrome cdkl5.xlsx
@@ -167,12 +167,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -506,6 +509,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
@@ -876,16 +880,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93168E3B-6BE7-4459-9C10-CE4A0A601E6B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b297ba6-3c75-43f4-b046-b7dedaa9211e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4b297ba6-3c75-43f4-b046-b7dedaa9211e"/>
     <ds:schemaRef ds:uri="d3de4b96-056f-41d8-923d-53addee4e8b2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>